<commit_message>
11/15/2016 Added Streamreader examples in Chapter Methods.
</commit_message>
<xml_diff>
--- a/I. Software Technologies & Design - Group 1A/STD 1A - results.xlsx
+++ b/I. Software Technologies & Design - Group 1A/STD 1A - results.xlsx
@@ -134,8 +134,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
   <autoFilter ref="A1:C20"/>
-  <sortState ref="A2:C20">
-    <sortCondition ref="A1:A20"/>
+  <sortState ref="A2:C19">
+    <sortCondition ref="B1:B20"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Име"/>
@@ -435,9 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -460,21 +458,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>1601681018</v>
+        <v>1601681001</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>1601681021</v>
+        <v>1601681005</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -482,35 +480,35 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>1601681020</v>
+        <v>1601681006</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>1601681015</v>
+        <v>1601681007</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1601681005</v>
+        <v>1601681008</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -526,10 +524,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>1601681001</v>
+        <v>1601681010</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -537,10 +535,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>1601681006</v>
+        <v>1601681011</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -548,10 +546,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>1601681019</v>
+        <v>1601681012</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -559,13 +557,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>1601681010</v>
+        <v>1601681013</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -581,13 +579,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>1601681013</v>
+        <v>1601681015</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -603,10 +601,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>1601681008</v>
+        <v>1601681017</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -614,10 +612,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>1601681017</v>
+        <v>1601681018</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -625,35 +623,35 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>1601681007</v>
+        <v>1601681019</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>1601681011</v>
+        <v>1601681020</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>1601681012</v>
+        <v>1601681021</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Exercises 2 results 23.11.2016
</commit_message>
<xml_diff>
--- a/I. Software Technologies & Design - Group 1A/STD 1A - results.xlsx
+++ b/I. Software Technologies & Design - Group 1A/STD 1A - results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Име</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Обща оценка</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -118,8 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +146,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0">
   <autoFilter ref="A1:E20"/>
-  <sortState ref="A2:C19">
+  <sortState ref="A2:E19">
     <sortCondition ref="B1:B20"/>
   </sortState>
   <tableColumns count="5">
@@ -444,7 +450,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,6 +489,12 @@
       <c r="C2">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -494,6 +506,12 @@
       <c r="C3">
         <v>6</v>
       </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -505,6 +523,12 @@
       <c r="C4">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -516,6 +540,12 @@
       <c r="C5">
         <v>6</v>
       </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -527,6 +557,12 @@
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -538,6 +574,12 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -549,6 +591,12 @@
       <c r="C8">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -560,6 +608,12 @@
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -571,6 +625,12 @@
       <c r="C10">
         <v>3</v>
       </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -581,6 +641,12 @@
       </c>
       <c r="C11">
         <v>4</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -593,6 +659,12 @@
       <c r="C12">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -604,6 +676,12 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -615,6 +693,12 @@
       <c r="C14">
         <v>4</v>
       </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -626,6 +710,12 @@
       <c r="C15">
         <v>4</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -637,8 +727,14 @@
       <c r="C16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -648,8 +744,14 @@
       <c r="C17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -659,8 +761,14 @@
       <c r="C18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -668,6 +776,12 @@
         <v>1601681021</v>
       </c>
       <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
         <v>6</v>
       </c>
     </row>

</xml_diff>